<commit_message>
adding momentum indicator as well
</commit_message>
<xml_diff>
--- a/portfolios/portfolio.xlsx
+++ b/portfolios/portfolio.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K100"/>
+  <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,27 +487,37 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>MACD</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Signal</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Momentum</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>RSI signal</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>MA signal</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>MACD</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Signal</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>MACD Signal</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Momentum Signal</t>
         </is>
       </c>
     </row>
@@ -534,23 +544,31 @@
       <c r="F2" t="n">
         <v>61.96428678473706</v>
       </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G2" t="n">
+        <v>1.167263978051295</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.6054055665690726</v>
       </c>
       <c r="I2" t="n">
-        <v>1.167263978051295</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.6054055665690726</v>
-      </c>
-      <c r="K2" s="3" t="inlineStr">
+        <v>1.080239338842784</v>
+      </c>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L2" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M2" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -579,25 +597,33 @@
       <c r="F3" t="n">
         <v>46.2834476104637</v>
       </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G3" t="n">
+        <v>0.3161585843020305</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.110502653856231</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3161585843020305</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1.110502653856231</v>
-      </c>
-      <c r="K3" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.118819899232568</v>
+      </c>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L3" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -624,25 +650,33 @@
       <c r="F4" t="n">
         <v>45.96717672691945</v>
       </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G4" t="n">
+        <v>0.5981797249991132</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.278742458678598</v>
       </c>
       <c r="I4" t="n">
-        <v>0.5981797249991132</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1.278742458678598</v>
-      </c>
-      <c r="K4" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.084881141218171</v>
+      </c>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L4" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M4" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -669,23 +703,31 @@
       <c r="F5" t="n">
         <v>33.09637299021556</v>
       </c>
-      <c r="G5" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H5" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G5" t="n">
+        <v>-10.44587390987783</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-6.379760633203002</v>
       </c>
       <c r="I5" t="n">
-        <v>-10.44587390987783</v>
-      </c>
-      <c r="J5" t="n">
-        <v>-6.379760633203002</v>
-      </c>
-      <c r="K5" s="4" t="inlineStr">
+        <v>0.9277100213613168</v>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L5" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M5" s="4" t="inlineStr">
         <is>
           <t>Sell</t>
         </is>
@@ -714,25 +756,33 @@
       <c r="F6" t="n">
         <v>59.34024769976354</v>
       </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G6" t="n">
+        <v>2.763807013378994</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3.781731321244157</v>
       </c>
       <c r="I6" t="n">
-        <v>2.763807013378994</v>
-      </c>
-      <c r="J6" t="n">
-        <v>3.781731321244157</v>
-      </c>
-      <c r="K6" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.149733922111583</v>
+      </c>
+      <c r="J6" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L6" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M6" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -759,25 +809,33 @@
       <c r="F7" t="n">
         <v>81.06952433097271</v>
       </c>
-      <c r="G7" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H7" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G7" t="n">
+        <v>0.5656684222625188</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-2.486396256070291</v>
       </c>
       <c r="I7" t="n">
-        <v>0.5656684222625188</v>
-      </c>
-      <c r="J7" t="n">
-        <v>-2.486396256070291</v>
-      </c>
-      <c r="K7" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.8882155842672894</v>
+      </c>
+      <c r="J7" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M7" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -804,23 +862,31 @@
       <c r="F8" t="n">
         <v>88.75114592510994</v>
       </c>
-      <c r="G8" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H8" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G8" t="n">
+        <v>4.004716115735533</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.955620752995722</v>
       </c>
       <c r="I8" t="n">
-        <v>4.004716115735533</v>
-      </c>
-      <c r="J8" t="n">
-        <v>1.955620752995722</v>
-      </c>
-      <c r="K8" s="3" t="inlineStr">
+        <v>1.032550388759989</v>
+      </c>
+      <c r="J8" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K8" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L8" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M8" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -849,25 +915,33 @@
       <c r="F9" t="n">
         <v>48.60953437232427</v>
       </c>
-      <c r="G9" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H9" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G9" t="n">
+        <v>-0.5485135242529964</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.03816933369286</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.5485135242529964</v>
-      </c>
-      <c r="J9" t="n">
-        <v>1.03816933369286</v>
-      </c>
-      <c r="K9" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.021283384978964</v>
+      </c>
+      <c r="J9" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K9" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L9" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M9" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -894,25 +968,33 @@
       <c r="F10" t="n">
         <v>82.42043444208397</v>
       </c>
-      <c r="G10" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H10" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G10" t="n">
+        <v>4.159588280951027</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3.118393493641597</v>
       </c>
       <c r="I10" t="n">
-        <v>4.159588280951027</v>
-      </c>
-      <c r="J10" t="n">
-        <v>3.118393493641597</v>
-      </c>
-      <c r="K10" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.9891850124818078</v>
+      </c>
+      <c r="J10" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K10" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L10" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M10" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -939,25 +1021,33 @@
       <c r="F11" t="n">
         <v>71.32100249322629</v>
       </c>
-      <c r="G11" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H11" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G11" t="n">
+        <v>-14.53526967713549</v>
+      </c>
+      <c r="H11" t="n">
+        <v>-22.92679773974312</v>
       </c>
       <c r="I11" t="n">
-        <v>-14.53526967713549</v>
-      </c>
-      <c r="J11" t="n">
-        <v>-22.92679773974312</v>
-      </c>
-      <c r="K11" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.8334946845409827</v>
+      </c>
+      <c r="J11" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K11" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M11" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -984,23 +1074,31 @@
       <c r="F12" t="n">
         <v>88.66929471258452</v>
       </c>
-      <c r="G12" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H12" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G12" t="n">
+        <v>4.967628982114888</v>
+      </c>
+      <c r="H12" t="n">
+        <v>2.857071660703359</v>
       </c>
       <c r="I12" t="n">
-        <v>4.967628982114888</v>
-      </c>
-      <c r="J12" t="n">
-        <v>2.857071660703359</v>
-      </c>
-      <c r="K12" s="3" t="inlineStr">
+        <v>1.109228748410117</v>
+      </c>
+      <c r="J12" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K12" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L12" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M12" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -1029,23 +1127,31 @@
       <c r="F13" t="n">
         <v>75.53531974910476</v>
       </c>
-      <c r="G13" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H13" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G13" t="n">
+        <v>5.305334595616955</v>
+      </c>
+      <c r="H13" t="n">
+        <v>4.683788597275992</v>
       </c>
       <c r="I13" t="n">
-        <v>5.305334595616955</v>
-      </c>
-      <c r="J13" t="n">
-        <v>4.683788597275992</v>
-      </c>
-      <c r="K13" s="3" t="inlineStr">
+        <v>1.158065171074714</v>
+      </c>
+      <c r="J13" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K13" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L13" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M13" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -1074,25 +1180,33 @@
       <c r="F14" t="n">
         <v>56.73760831982857</v>
       </c>
-      <c r="G14" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H14" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G14" t="n">
+        <v>-0.0032524616430293</v>
+      </c>
+      <c r="H14" t="n">
+        <v>-0.0095715018544325</v>
       </c>
       <c r="I14" t="n">
-        <v>-0.0032524616430293</v>
-      </c>
-      <c r="J14" t="n">
-        <v>-0.0095715018544325</v>
-      </c>
-      <c r="K14" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.9937138547366751</v>
+      </c>
+      <c r="J14" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K14" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L14" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M14" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -1119,23 +1233,31 @@
       <c r="F15" t="n">
         <v>94.3666081013556</v>
       </c>
-      <c r="G15" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H15" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
+      <c r="G15" t="n">
+        <v>114.5938274552045</v>
+      </c>
+      <c r="H15" t="n">
+        <v>83.7537189746723</v>
       </c>
       <c r="I15" t="n">
-        <v>114.5938274552045</v>
-      </c>
-      <c r="J15" t="n">
-        <v>83.7537189746723</v>
-      </c>
-      <c r="K15" s="3" t="inlineStr">
+        <v>1.077606952267134</v>
+      </c>
+      <c r="J15" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K15" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L15" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M15" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -1164,25 +1286,33 @@
       <c r="F16" t="n">
         <v>58.53365098054319</v>
       </c>
-      <c r="G16" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H16" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G16" t="n">
+        <v>0.5838019749720473</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.5973181135946853</v>
       </c>
       <c r="I16" t="n">
-        <v>0.5838019749720473</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.5973181135946853</v>
-      </c>
-      <c r="K16" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.206838439804387</v>
+      </c>
+      <c r="J16" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K16" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L16" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M16" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -1209,23 +1339,31 @@
       <c r="F17" t="n">
         <v>76.32849671776515</v>
       </c>
-      <c r="G17" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H17" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G17" t="n">
+        <v>5.10582446346433</v>
+      </c>
+      <c r="H17" t="n">
+        <v>4.881062877181913</v>
       </c>
       <c r="I17" t="n">
-        <v>5.10582446346433</v>
-      </c>
-      <c r="J17" t="n">
-        <v>4.881062877181913</v>
-      </c>
-      <c r="K17" s="3" t="inlineStr">
+        <v>1.239660722435855</v>
+      </c>
+      <c r="J17" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K17" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L17" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M17" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -1254,25 +1392,33 @@
       <c r="F18" t="n">
         <v>59.87932788861779</v>
       </c>
-      <c r="G18" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H18" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G18" t="n">
+        <v>0.1558978432537756</v>
+      </c>
+      <c r="H18" t="n">
+        <v>-0.167748823951006</v>
       </c>
       <c r="I18" t="n">
-        <v>0.1558978432537756</v>
-      </c>
-      <c r="J18" t="n">
-        <v>-0.167748823951006</v>
-      </c>
-      <c r="K18" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.9724235735069812</v>
+      </c>
+      <c r="J18" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K18" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L18" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M18" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -1299,25 +1445,33 @@
       <c r="F19" t="n">
         <v>59.81012150857826</v>
       </c>
-      <c r="G19" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H19" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G19" t="n">
+        <v>0.0082008213409322</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.0096500479652093</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0082008213409322</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0.0096500479652093</v>
-      </c>
-      <c r="K19" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.039999961853027</v>
+      </c>
+      <c r="J19" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K19" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L19" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M19" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -1344,23 +1498,31 @@
       <c r="F20" t="n">
         <v>85.83897267159574</v>
       </c>
-      <c r="G20" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H20" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
+      <c r="G20" t="n">
+        <v>10.92062322820448</v>
+      </c>
+      <c r="H20" t="n">
+        <v>6.317660296613534</v>
       </c>
       <c r="I20" t="n">
-        <v>10.92062322820448</v>
-      </c>
-      <c r="J20" t="n">
-        <v>6.317660296613534</v>
-      </c>
-      <c r="K20" s="3" t="inlineStr">
+        <v>1.173701543954886</v>
+      </c>
+      <c r="J20" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K20" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L20" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M20" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -1389,23 +1551,31 @@
       <c r="F21" t="n">
         <v>62.01022235075075</v>
       </c>
-      <c r="G21" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H21" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G21" t="n">
+        <v>0.3489159060238691</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.1791720266228732</v>
       </c>
       <c r="I21" t="n">
-        <v>0.3489159060238691</v>
-      </c>
-      <c r="J21" t="n">
-        <v>0.1791720266228732</v>
-      </c>
-      <c r="K21" s="3" t="inlineStr">
+        <v>1.047497462145023</v>
+      </c>
+      <c r="J21" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K21" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L21" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M21" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -1434,23 +1604,31 @@
       <c r="F22" t="n">
         <v>40.56940012497154</v>
       </c>
-      <c r="G22" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H22" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
-        </is>
+      <c r="G22" t="n">
+        <v>-0.8864492728469457</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-0.7751088496389174</v>
       </c>
       <c r="I22" t="n">
-        <v>-0.8864492728469457</v>
-      </c>
-      <c r="J22" t="n">
-        <v>-0.7751088496389174</v>
-      </c>
-      <c r="K22" s="4" t="inlineStr">
+        <v>0.8944745586233741</v>
+      </c>
+      <c r="J22" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K22" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L22" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M22" s="4" t="inlineStr">
         <is>
           <t>Sell</t>
         </is>
@@ -1479,25 +1657,33 @@
       <c r="F23" t="n">
         <v>60.21789484183557</v>
       </c>
-      <c r="G23" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H23" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G23" t="n">
+        <v>9.313179756333623</v>
+      </c>
+      <c r="H23" t="n">
+        <v>10.69053014062218</v>
       </c>
       <c r="I23" t="n">
-        <v>9.313179756333623</v>
-      </c>
-      <c r="J23" t="n">
-        <v>10.69053014062218</v>
-      </c>
-      <c r="K23" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.06053013894063</v>
+      </c>
+      <c r="J23" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K23" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L23" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M23" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -1524,23 +1710,31 @@
       <c r="F24" t="n">
         <v>84.60700249495859</v>
       </c>
-      <c r="G24" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H24" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
+      <c r="G24" t="n">
+        <v>4.534152335192061</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.934324100298974</v>
       </c>
       <c r="I24" t="n">
-        <v>4.534152335192061</v>
-      </c>
-      <c r="J24" t="n">
-        <v>1.934324100298974</v>
-      </c>
-      <c r="K24" s="3" t="inlineStr">
+        <v>1.072578775648089</v>
+      </c>
+      <c r="J24" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K24" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L24" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M24" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -1569,25 +1763,33 @@
       <c r="F25" t="n">
         <v>73.38398309433055</v>
       </c>
-      <c r="G25" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H25" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G25" t="n">
+        <v>5.207117467551768</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1.714333292768755</v>
       </c>
       <c r="I25" t="n">
-        <v>5.207117467551768</v>
-      </c>
-      <c r="J25" t="n">
-        <v>1.714333292768755</v>
-      </c>
-      <c r="K25" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.7345703415875765</v>
+      </c>
+      <c r="J25" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K25" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L25" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M25" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -1614,23 +1816,31 @@
       <c r="F26" t="n">
         <v>91.27135906096136</v>
       </c>
-      <c r="G26" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H26" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
+      <c r="G26" t="n">
+        <v>1.02888905132501</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.8012487691570993</v>
       </c>
       <c r="I26" t="n">
-        <v>1.02888905132501</v>
-      </c>
-      <c r="J26" t="n">
-        <v>0.8012487691570993</v>
-      </c>
-      <c r="K26" s="3" t="inlineStr">
+        <v>1.112397397205708</v>
+      </c>
+      <c r="J26" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K26" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L26" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M26" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -1659,25 +1869,33 @@
       <c r="F27" t="n">
         <v>57.51790247741791</v>
       </c>
-      <c r="G27" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H27" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G27" t="n">
+        <v>0.1196239885051824</v>
+      </c>
+      <c r="H27" t="n">
+        <v>-0.0383849194728327</v>
       </c>
       <c r="I27" t="n">
-        <v>0.1196239885051824</v>
-      </c>
-      <c r="J27" t="n">
-        <v>-0.0383849194728327</v>
-      </c>
-      <c r="K27" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.9991533516661849</v>
+      </c>
+      <c r="J27" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K27" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L27" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M27" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -1704,25 +1922,33 @@
       <c r="F28" t="n">
         <v>58.85392746829091</v>
       </c>
-      <c r="G28" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H28" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G28" t="n">
+        <v>-0.5117601331303661</v>
+      </c>
+      <c r="H28" t="n">
+        <v>-1.085311754860729</v>
       </c>
       <c r="I28" t="n">
-        <v>-0.5117601331303661</v>
-      </c>
-      <c r="J28" t="n">
-        <v>-1.085311754860729</v>
-      </c>
-      <c r="K28" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.9077484155178434</v>
+      </c>
+      <c r="J28" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K28" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L28" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M28" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -1749,23 +1975,31 @@
       <c r="F29" t="n">
         <v>80.68951048513105</v>
       </c>
-      <c r="G29" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H29" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G29" t="n">
+        <v>9.472977935295605</v>
+      </c>
+      <c r="H29" t="n">
+        <v>8.337528009282895</v>
       </c>
       <c r="I29" t="n">
-        <v>9.472977935295605</v>
-      </c>
-      <c r="J29" t="n">
-        <v>8.337528009282895</v>
-      </c>
-      <c r="K29" s="3" t="inlineStr">
+        <v>1.101276652954462</v>
+      </c>
+      <c r="J29" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K29" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L29" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M29" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -1794,25 +2028,33 @@
       <c r="F30" t="n">
         <v>61.99954131446169</v>
       </c>
-      <c r="G30" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H30" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G30" t="n">
+        <v>1.75813305737978</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1.858110351420534</v>
       </c>
       <c r="I30" t="n">
-        <v>1.75813305737978</v>
-      </c>
-      <c r="J30" t="n">
-        <v>1.858110351420534</v>
-      </c>
-      <c r="K30" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.108384974627722</v>
+      </c>
+      <c r="J30" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K30" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L30" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M30" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -1839,25 +2081,33 @@
       <c r="F31" t="n">
         <v>89.2856612055427</v>
       </c>
-      <c r="G31" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H31" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G31" t="n">
+        <v>1.09986117704311</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0.5654973850124327</v>
       </c>
       <c r="I31" t="n">
-        <v>1.09986117704311</v>
-      </c>
-      <c r="J31" t="n">
-        <v>0.5654973850124327</v>
-      </c>
-      <c r="K31" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.9588074939110457</v>
+      </c>
+      <c r="J31" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K31" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L31" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M31" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -1884,23 +2134,31 @@
       <c r="F32" t="n">
         <v>28.39165921765228</v>
       </c>
-      <c r="G32" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
-        </is>
-      </c>
-      <c r="H32" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G32" t="n">
+        <v>-3.822071530334711</v>
+      </c>
+      <c r="H32" t="n">
+        <v>-0.323057070901566</v>
       </c>
       <c r="I32" t="n">
-        <v>-3.822071530334711</v>
-      </c>
-      <c r="J32" t="n">
-        <v>-0.323057070901566</v>
-      </c>
-      <c r="K32" s="4" t="inlineStr">
+        <v>0.9601742947660432</v>
+      </c>
+      <c r="J32" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="K32" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L32" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M32" s="4" t="inlineStr">
         <is>
           <t>Sell</t>
         </is>
@@ -1929,23 +2187,31 @@
       <c r="F33" t="n">
         <v>92.42449554118984</v>
       </c>
-      <c r="G33" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H33" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G33" t="n">
+        <v>9.116972264142476</v>
+      </c>
+      <c r="H33" t="n">
+        <v>5.799934615352232</v>
       </c>
       <c r="I33" t="n">
-        <v>9.116972264142476</v>
-      </c>
-      <c r="J33" t="n">
-        <v>5.799934615352232</v>
-      </c>
-      <c r="K33" s="3" t="inlineStr">
+        <v>1.062095365902418</v>
+      </c>
+      <c r="J33" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K33" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L33" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M33" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -1974,23 +2240,31 @@
       <c r="F34" t="n">
         <v>39.74971554755832</v>
       </c>
-      <c r="G34" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H34" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
-        </is>
+      <c r="G34" t="n">
+        <v>-6.51671884012211</v>
+      </c>
+      <c r="H34" t="n">
+        <v>-3.731603859013528</v>
       </c>
       <c r="I34" t="n">
-        <v>-6.51671884012211</v>
-      </c>
-      <c r="J34" t="n">
-        <v>-3.731603859013528</v>
-      </c>
-      <c r="K34" s="4" t="inlineStr">
+        <v>0.8882403609428328</v>
+      </c>
+      <c r="J34" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K34" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="L34" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M34" s="4" t="inlineStr">
         <is>
           <t>Sell</t>
         </is>
@@ -2019,23 +2293,31 @@
       <c r="F35" t="n">
         <v>81.58464482049052</v>
       </c>
-      <c r="G35" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H35" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G35" t="n">
+        <v>5.494879737199909</v>
+      </c>
+      <c r="H35" t="n">
+        <v>4.260598932481348</v>
       </c>
       <c r="I35" t="n">
-        <v>5.494879737199909</v>
-      </c>
-      <c r="J35" t="n">
-        <v>4.260598932481348</v>
-      </c>
-      <c r="K35" s="3" t="inlineStr">
+        <v>1.161162451534604</v>
+      </c>
+      <c r="J35" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K35" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L35" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M35" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -2064,23 +2346,31 @@
       <c r="F36" t="n">
         <v>83.9070726479093</v>
       </c>
-      <c r="G36" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H36" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
+      <c r="G36" t="n">
+        <v>4.371756810410261</v>
+      </c>
+      <c r="H36" t="n">
+        <v>3.437604877232423</v>
       </c>
       <c r="I36" t="n">
-        <v>4.371756810410261</v>
-      </c>
-      <c r="J36" t="n">
-        <v>3.437604877232423</v>
-      </c>
-      <c r="K36" s="3" t="inlineStr">
+        <v>1.148690768045606</v>
+      </c>
+      <c r="J36" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K36" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L36" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M36" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -2109,25 +2399,33 @@
       <c r="F37" t="n">
         <v>77.43902744507514</v>
       </c>
-      <c r="G37" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H37" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G37" t="n">
+        <v>-0.3967138472127089</v>
+      </c>
+      <c r="H37" t="n">
+        <v>-1.675569726226815</v>
       </c>
       <c r="I37" t="n">
-        <v>-0.3967138472127089</v>
-      </c>
-      <c r="J37" t="n">
-        <v>-1.675569726226815</v>
-      </c>
-      <c r="K37" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.8931959626351834</v>
+      </c>
+      <c r="J37" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K37" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L37" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M37" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -2154,25 +2452,33 @@
       <c r="F38" t="n">
         <v>77.58063803432631</v>
       </c>
-      <c r="G38" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H38" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G38" t="n">
+        <v>-0.3082216310671697</v>
+      </c>
+      <c r="H38" t="n">
+        <v>-1.544992513363707</v>
       </c>
       <c r="I38" t="n">
-        <v>-0.3082216310671697</v>
-      </c>
-      <c r="J38" t="n">
-        <v>-1.544992513363707</v>
-      </c>
-      <c r="K38" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.8933845796339598</v>
+      </c>
+      <c r="J38" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K38" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M38" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -2199,23 +2505,31 @@
       <c r="F39" t="n">
         <v>59.7896320320992</v>
       </c>
-      <c r="G39" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H39" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G39" t="n">
+        <v>1.271278088868087</v>
+      </c>
+      <c r="H39" t="n">
+        <v>-0.0156401111570039</v>
       </c>
       <c r="I39" t="n">
-        <v>1.271278088868087</v>
-      </c>
-      <c r="J39" t="n">
-        <v>-0.0156401111570039</v>
-      </c>
-      <c r="K39" s="3" t="inlineStr">
+        <v>1.098602771005764</v>
+      </c>
+      <c r="J39" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K39" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L39" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M39" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -2244,23 +2558,31 @@
       <c r="F40" t="n">
         <v>89.58737684858968</v>
       </c>
-      <c r="G40" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H40" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
+      <c r="G40" t="n">
+        <v>9.010088955988069</v>
+      </c>
+      <c r="H40" t="n">
+        <v>7.138479497058844</v>
       </c>
       <c r="I40" t="n">
-        <v>9.010088955988069</v>
-      </c>
-      <c r="J40" t="n">
-        <v>7.138479497058844</v>
-      </c>
-      <c r="K40" s="3" t="inlineStr">
+        <v>1.152393746981398</v>
+      </c>
+      <c r="J40" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K40" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M40" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -2289,25 +2611,33 @@
       <c r="F41" t="n">
         <v>75.96266667616261</v>
       </c>
-      <c r="G41" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H41" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G41" t="n">
+        <v>0.5455570086577382</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0.0853149483401331</v>
       </c>
       <c r="I41" t="n">
-        <v>0.5455570086577382</v>
-      </c>
-      <c r="J41" t="n">
-        <v>0.0853149483401331</v>
-      </c>
-      <c r="K41" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.9695139331670163</v>
+      </c>
+      <c r="J41" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K41" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L41" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M41" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -2334,23 +2664,31 @@
       <c r="F42" t="n">
         <v>86.77470650934694</v>
       </c>
-      <c r="G42" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H42" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
+      <c r="G42" t="n">
+        <v>6.921510015483335</v>
+      </c>
+      <c r="H42" t="n">
+        <v>6.246130033699969</v>
       </c>
       <c r="I42" t="n">
-        <v>6.921510015483335</v>
-      </c>
-      <c r="J42" t="n">
-        <v>6.246130033699969</v>
-      </c>
-      <c r="K42" s="3" t="inlineStr">
+        <v>1.291876245263224</v>
+      </c>
+      <c r="J42" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K42" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L42" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M42" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -2379,25 +2717,33 @@
       <c r="F43" t="n">
         <v>85.07673158483198</v>
       </c>
-      <c r="G43" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H43" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G43" t="n">
+        <v>0.2319582036567915</v>
+      </c>
+      <c r="H43" t="n">
+        <v>-0.4293929989442629</v>
       </c>
       <c r="I43" t="n">
-        <v>0.2319582036567915</v>
-      </c>
-      <c r="J43" t="n">
-        <v>-0.4293929989442629</v>
-      </c>
-      <c r="K43" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.7723603683122934</v>
+      </c>
+      <c r="J43" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K43" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L43" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M43" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -2424,23 +2770,31 @@
       <c r="F44" t="n">
         <v>60.31943220305055</v>
       </c>
-      <c r="G44" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H44" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G44" t="n">
+        <v>1.070493836817604</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1.232876126070837</v>
       </c>
       <c r="I44" t="n">
-        <v>1.070493836817604</v>
-      </c>
-      <c r="J44" t="n">
-        <v>1.232876126070837</v>
-      </c>
-      <c r="K44" s="4" t="inlineStr">
+        <v>0.9689901185291717</v>
+      </c>
+      <c r="J44" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K44" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L44" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M44" s="4" t="inlineStr">
         <is>
           <t>Sell</t>
         </is>
@@ -2469,23 +2823,31 @@
       <c r="F45" t="n">
         <v>85.50328660806208</v>
       </c>
-      <c r="G45" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H45" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G45" t="n">
+        <v>5.689910960898828</v>
+      </c>
+      <c r="H45" t="n">
+        <v>4.526355065914159</v>
       </c>
       <c r="I45" t="n">
-        <v>5.689910960898828</v>
-      </c>
-      <c r="J45" t="n">
-        <v>4.526355065914159</v>
-      </c>
-      <c r="K45" s="3" t="inlineStr">
+        <v>1.050947509964514</v>
+      </c>
+      <c r="J45" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K45" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L45" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M45" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -2514,23 +2876,31 @@
       <c r="F46" t="n">
         <v>72.265148939022</v>
       </c>
-      <c r="G46" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H46" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G46" t="n">
+        <v>1.877605989793807</v>
+      </c>
+      <c r="H46" t="n">
+        <v>1.537490336558349</v>
       </c>
       <c r="I46" t="n">
-        <v>1.877605989793807</v>
-      </c>
-      <c r="J46" t="n">
-        <v>1.537490336558349</v>
-      </c>
-      <c r="K46" s="3" t="inlineStr">
+        <v>1.078663348424661</v>
+      </c>
+      <c r="J46" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K46" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L46" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M46" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -2559,25 +2929,33 @@
       <c r="F47" t="n">
         <v>40.311069489261</v>
       </c>
-      <c r="G47" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H47" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G47" t="n">
+        <v>0.2290941566102162</v>
+      </c>
+      <c r="H47" t="n">
+        <v>1.111176192150155</v>
       </c>
       <c r="I47" t="n">
-        <v>0.2290941566102162</v>
-      </c>
-      <c r="J47" t="n">
-        <v>1.111176192150155</v>
-      </c>
-      <c r="K47" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.104200843910401</v>
+      </c>
+      <c r="J47" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K47" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L47" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M47" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -2604,25 +2982,33 @@
       <c r="F48" t="n">
         <v>45.90212433359387</v>
       </c>
-      <c r="G48" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H48" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G48" t="n">
+        <v>-0.7425117228653733</v>
+      </c>
+      <c r="H48" t="n">
+        <v>-0.5852380813956723</v>
       </c>
       <c r="I48" t="n">
-        <v>-0.7425117228653733</v>
-      </c>
-      <c r="J48" t="n">
-        <v>-0.5852380813956723</v>
-      </c>
-      <c r="K48" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.037179889630654</v>
+      </c>
+      <c r="J48" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K48" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L48" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M48" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -2649,25 +3035,33 @@
       <c r="F49" t="n">
         <v>52.29684646128339</v>
       </c>
-      <c r="G49" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H49" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G49" t="n">
+        <v>0.5101114453412663</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.7091781984196606</v>
       </c>
       <c r="I49" t="n">
-        <v>0.5101114453412663</v>
-      </c>
-      <c r="J49" t="n">
-        <v>0.7091781984196606</v>
-      </c>
-      <c r="K49" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.121759620019003</v>
+      </c>
+      <c r="J49" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K49" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L49" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M49" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -2694,23 +3088,31 @@
       <c r="F50" t="n">
         <v>77.42433465663839</v>
       </c>
-      <c r="G50" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H50" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G50" t="n">
+        <v>4.992425429143452</v>
+      </c>
+      <c r="H50" t="n">
+        <v>4.384165336860001</v>
       </c>
       <c r="I50" t="n">
-        <v>4.992425429143452</v>
-      </c>
-      <c r="J50" t="n">
-        <v>4.384165336860001</v>
-      </c>
-      <c r="K50" s="3" t="inlineStr">
+        <v>1.097696030983121</v>
+      </c>
+      <c r="J50" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K50" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L50" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M50" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -2739,25 +3141,33 @@
       <c r="F51" t="n">
         <v>52.82068058054482</v>
       </c>
-      <c r="G51" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H51" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G51" t="n">
+        <v>1.671192097687026</v>
+      </c>
+      <c r="H51" t="n">
+        <v>3.905878665421938</v>
       </c>
       <c r="I51" t="n">
-        <v>1.671192097687026</v>
-      </c>
-      <c r="J51" t="n">
-        <v>3.905878665421938</v>
-      </c>
-      <c r="K51" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.004351766573325</v>
+      </c>
+      <c r="J51" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K51" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L51" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M51" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -2784,25 +3194,33 @@
       <c r="F52" t="n">
         <v>60.41790650003306</v>
       </c>
-      <c r="G52" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H52" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G52" t="n">
+        <v>7.126397151222591</v>
+      </c>
+      <c r="H52" t="n">
+        <v>7.814858311652907</v>
       </c>
       <c r="I52" t="n">
-        <v>7.126397151222591</v>
-      </c>
-      <c r="J52" t="n">
-        <v>7.814858311652907</v>
-      </c>
-      <c r="K52" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.236137908090934</v>
+      </c>
+      <c r="J52" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K52" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L52" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M52" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -2829,23 +3247,31 @@
       <c r="F53" t="n">
         <v>92.18269471516102</v>
       </c>
-      <c r="G53" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H53" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G53" t="n">
+        <v>6.086386290786834</v>
+      </c>
+      <c r="H53" t="n">
+        <v>5.065432921508379</v>
       </c>
       <c r="I53" t="n">
-        <v>6.086386290786834</v>
-      </c>
-      <c r="J53" t="n">
-        <v>5.065432921508379</v>
-      </c>
-      <c r="K53" s="3" t="inlineStr">
+        <v>1.204798953382484</v>
+      </c>
+      <c r="J53" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K53" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L53" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M53" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -2874,25 +3300,33 @@
       <c r="F54" t="n">
         <v>74.50736404331917</v>
       </c>
-      <c r="G54" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H54" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G54" t="n">
+        <v>-7.26357974366033</v>
+      </c>
+      <c r="H54" t="n">
+        <v>-20.17414716335407</v>
       </c>
       <c r="I54" t="n">
-        <v>-7.26357974366033</v>
-      </c>
-      <c r="J54" t="n">
-        <v>-20.17414716335407</v>
-      </c>
-      <c r="K54" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.7958867628593973</v>
+      </c>
+      <c r="J54" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K54" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L54" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M54" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -2919,25 +3353,33 @@
       <c r="F55" t="n">
         <v>64.82096379628761</v>
       </c>
-      <c r="G55" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H55" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G55" t="n">
+        <v>6.585796951054704</v>
+      </c>
+      <c r="H55" t="n">
+        <v>7.953436239135995</v>
       </c>
       <c r="I55" t="n">
-        <v>6.585796951054704</v>
-      </c>
-      <c r="J55" t="n">
-        <v>7.953436239135995</v>
-      </c>
-      <c r="K55" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.113586873097278</v>
+      </c>
+      <c r="J55" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K55" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L55" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M55" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -2964,23 +3406,31 @@
       <c r="F56" t="n">
         <v>77.63876378690178</v>
       </c>
-      <c r="G56" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H56" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G56" t="n">
+        <v>5.632552037850985</v>
+      </c>
+      <c r="H56" t="n">
+        <v>5.442870949930615</v>
       </c>
       <c r="I56" t="n">
-        <v>5.632552037850985</v>
-      </c>
-      <c r="J56" t="n">
-        <v>5.442870949930615</v>
-      </c>
-      <c r="K56" s="3" t="inlineStr">
+        <v>1.191531934782627</v>
+      </c>
+      <c r="J56" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K56" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L56" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M56" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -3009,25 +3459,33 @@
       <c r="F57" t="n">
         <v>40.57146261820095</v>
       </c>
-      <c r="G57" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H57" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G57" t="n">
+        <v>0.905332921959456</v>
+      </c>
+      <c r="H57" t="n">
+        <v>1.204436484166528</v>
       </c>
       <c r="I57" t="n">
-        <v>0.905332921959456</v>
-      </c>
-      <c r="J57" t="n">
-        <v>1.204436484166528</v>
-      </c>
-      <c r="K57" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.135696774482381</v>
+      </c>
+      <c r="J57" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K57" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L57" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M57" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -3054,25 +3512,33 @@
       <c r="F58" t="n">
         <v>46.71640567352628</v>
       </c>
-      <c r="G58" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H58" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G58" t="n">
+        <v>1.028359673625673</v>
+      </c>
+      <c r="H58" t="n">
+        <v>1.380131111355849</v>
       </c>
       <c r="I58" t="n">
-        <v>1.028359673625673</v>
-      </c>
-      <c r="J58" t="n">
-        <v>1.380131111355849</v>
-      </c>
-      <c r="K58" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.136450234896372</v>
+      </c>
+      <c r="J58" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K58" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L58" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M58" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -3099,23 +3565,31 @@
       <c r="F59" t="n">
         <v>96.51671159086276</v>
       </c>
-      <c r="G59" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H59" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G59" t="n">
+        <v>14.48231253560709</v>
+      </c>
+      <c r="H59" t="n">
+        <v>10.22223548573819</v>
       </c>
       <c r="I59" t="n">
-        <v>14.48231253560709</v>
-      </c>
-      <c r="J59" t="n">
-        <v>10.22223548573819</v>
-      </c>
-      <c r="K59" s="3" t="inlineStr">
+        <v>1.126175132840314</v>
+      </c>
+      <c r="J59" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K59" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L59" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M59" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -3144,23 +3618,31 @@
       <c r="F60" t="n">
         <v>31.16574238663907</v>
       </c>
-      <c r="G60" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H60" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G60" t="n">
+        <v>-0.5772737567164512</v>
+      </c>
+      <c r="H60" t="n">
+        <v>-0.3110689460218745</v>
       </c>
       <c r="I60" t="n">
-        <v>-0.5772737567164512</v>
-      </c>
-      <c r="J60" t="n">
-        <v>-0.3110689460218745</v>
-      </c>
-      <c r="K60" s="4" t="inlineStr">
+        <v>0.9134894470932317</v>
+      </c>
+      <c r="J60" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K60" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L60" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M60" s="4" t="inlineStr">
         <is>
           <t>Sell</t>
         </is>
@@ -3189,23 +3671,31 @@
       <c r="F61" t="n">
         <v>78.66859631637153</v>
       </c>
-      <c r="G61" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H61" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G61" t="n">
+        <v>0.8401815109406954</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.2634248108865201</v>
       </c>
       <c r="I61" t="n">
-        <v>0.8401815109406954</v>
-      </c>
-      <c r="J61" t="n">
-        <v>0.2634248108865201</v>
-      </c>
-      <c r="K61" s="3" t="inlineStr">
+        <v>1.076242369035665</v>
+      </c>
+      <c r="J61" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K61" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L61" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M61" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -3234,25 +3724,33 @@
       <c r="F62" t="n">
         <v>75.12304403485004</v>
       </c>
-      <c r="G62" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H62" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G62" t="n">
+        <v>4.092365158025302</v>
+      </c>
+      <c r="H62" t="n">
+        <v>2.984787282454053</v>
       </c>
       <c r="I62" t="n">
-        <v>4.092365158025302</v>
-      </c>
-      <c r="J62" t="n">
-        <v>2.984787282454053</v>
-      </c>
-      <c r="K62" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.9650072396883771</v>
+      </c>
+      <c r="J62" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K62" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L62" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M62" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -3279,25 +3777,33 @@
       <c r="F63" t="n">
         <v>78.35423499335189</v>
       </c>
-      <c r="G63" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H63" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G63" t="n">
+        <v>-0.4415197650584446</v>
+      </c>
+      <c r="H63" t="n">
+        <v>-2.866851195648449</v>
       </c>
       <c r="I63" t="n">
-        <v>-0.4415197650584446</v>
-      </c>
-      <c r="J63" t="n">
-        <v>-2.866851195648449</v>
-      </c>
-      <c r="K63" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.8353987552131972</v>
+      </c>
+      <c r="J63" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K63" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L63" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M63" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -3324,25 +3830,33 @@
       <c r="F64" t="n">
         <v>64.21566244182901</v>
       </c>
-      <c r="G64" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H64" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G64" t="n">
+        <v>1.476891143655052</v>
+      </c>
+      <c r="H64" t="n">
+        <v>1.611224427711716</v>
       </c>
       <c r="I64" t="n">
-        <v>1.476891143655052</v>
-      </c>
-      <c r="J64" t="n">
-        <v>1.611224427711716</v>
-      </c>
-      <c r="K64" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.178647111453595</v>
+      </c>
+      <c r="J64" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K64" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L64" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M64" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -3369,23 +3883,31 @@
       <c r="F65" t="n">
         <v>70.47533548826783</v>
       </c>
-      <c r="G65" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H65" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G65" t="n">
+        <v>11.97292482237742</v>
+      </c>
+      <c r="H65" t="n">
+        <v>10.26244051258228</v>
       </c>
       <c r="I65" t="n">
-        <v>11.97292482237742</v>
-      </c>
-      <c r="J65" t="n">
-        <v>10.26244051258228</v>
-      </c>
-      <c r="K65" s="3" t="inlineStr">
+        <v>1.054157757717708</v>
+      </c>
+      <c r="J65" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K65" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L65" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M65" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -3414,23 +3936,31 @@
       <c r="F66" t="n">
         <v>80.24861914840591</v>
       </c>
-      <c r="G66" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H66" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
+      <c r="G66" t="n">
+        <v>2.134063581723922</v>
+      </c>
+      <c r="H66" t="n">
+        <v>1.301576713899196</v>
       </c>
       <c r="I66" t="n">
-        <v>2.134063581723922</v>
-      </c>
-      <c r="J66" t="n">
-        <v>1.301576713899196</v>
-      </c>
-      <c r="K66" s="3" t="inlineStr">
+        <v>1.18601560477855</v>
+      </c>
+      <c r="J66" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K66" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L66" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M66" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -3459,25 +3989,33 @@
       <c r="F67" t="n">
         <v>65.5425084611586</v>
       </c>
-      <c r="G67" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H67" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G67" t="n">
+        <v>22.66493791014307</v>
+      </c>
+      <c r="H67" t="n">
+        <v>23.12847544558373</v>
       </c>
       <c r="I67" t="n">
-        <v>22.66493791014307</v>
-      </c>
-      <c r="J67" t="n">
-        <v>23.12847544558373</v>
-      </c>
-      <c r="K67" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.124817273538477</v>
+      </c>
+      <c r="J67" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K67" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L67" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M67" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -3504,23 +4042,31 @@
       <c r="F68" t="n">
         <v>79.06275736663142</v>
       </c>
-      <c r="G68" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H68" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G68" t="n">
+        <v>1.123764154612218</v>
+      </c>
+      <c r="H68" t="n">
+        <v>-0.0546934702894807</v>
       </c>
       <c r="I68" t="n">
-        <v>1.123764154612218</v>
-      </c>
-      <c r="J68" t="n">
-        <v>-0.0546934702894807</v>
-      </c>
-      <c r="K68" s="3" t="inlineStr">
+        <v>1.004047272108585</v>
+      </c>
+      <c r="J68" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K68" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L68" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M68" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -3549,23 +4095,31 @@
       <c r="F69" t="n">
         <v>40.2508651572594</v>
       </c>
-      <c r="G69" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H69" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G69" t="n">
+        <v>-2.187786448067641</v>
+      </c>
+      <c r="H69" t="n">
+        <v>-1.11379732926335</v>
       </c>
       <c r="I69" t="n">
-        <v>-2.187786448067641</v>
-      </c>
-      <c r="J69" t="n">
-        <v>-1.11379732926335</v>
-      </c>
-      <c r="K69" s="4" t="inlineStr">
+        <v>0.8708140554030638</v>
+      </c>
+      <c r="J69" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K69" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L69" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M69" s="4" t="inlineStr">
         <is>
           <t>Sell</t>
         </is>
@@ -3594,23 +4148,31 @@
       <c r="F70" t="n">
         <v>78.49556228284428</v>
       </c>
-      <c r="G70" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H70" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
+      <c r="G70" t="n">
+        <v>7.482246987928335</v>
+      </c>
+      <c r="H70" t="n">
+        <v>6.964127512403115</v>
       </c>
       <c r="I70" t="n">
-        <v>7.482246987928335</v>
-      </c>
-      <c r="J70" t="n">
-        <v>6.964127512403115</v>
-      </c>
-      <c r="K70" s="3" t="inlineStr">
+        <v>1.190509983970707</v>
+      </c>
+      <c r="J70" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K70" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L70" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M70" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -3639,23 +4201,31 @@
       <c r="F71" t="n">
         <v>52.43678117446949</v>
       </c>
-      <c r="G71" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H71" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G71" t="n">
+        <v>-0.3187745504221198</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0.5333255200894718</v>
       </c>
       <c r="I71" t="n">
-        <v>-0.3187745504221198</v>
-      </c>
-      <c r="J71" t="n">
-        <v>0.5333255200894718</v>
-      </c>
-      <c r="K71" s="4" t="inlineStr">
+        <v>0.9991740692863599</v>
+      </c>
+      <c r="J71" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K71" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L71" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M71" s="4" t="inlineStr">
         <is>
           <t>Sell</t>
         </is>
@@ -3684,25 +4254,33 @@
       <c r="F72" t="n">
         <v>24.41480925037203</v>
       </c>
-      <c r="G72" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
-        </is>
-      </c>
-      <c r="H72" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G72" t="n">
+        <v>-0.9326089067638748</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0.1218518803823435</v>
       </c>
       <c r="I72" t="n">
-        <v>-0.9326089067638748</v>
-      </c>
-      <c r="J72" t="n">
-        <v>0.1218518803823435</v>
-      </c>
-      <c r="K72" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.028860789286411</v>
+      </c>
+      <c r="J72" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="K72" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L72" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M72" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -3729,25 +4307,33 @@
       <c r="F73" t="n">
         <v>54.84633441822253</v>
       </c>
-      <c r="G73" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H73" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G73" t="n">
+        <v>0.0620810248844883</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0.1081198738236505</v>
       </c>
       <c r="I73" t="n">
-        <v>0.0620810248844883</v>
-      </c>
-      <c r="J73" t="n">
-        <v>0.1081198738236505</v>
-      </c>
-      <c r="K73" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.035382408410112</v>
+      </c>
+      <c r="J73" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K73" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L73" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M73" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -3774,25 +4360,33 @@
       <c r="F74" t="n">
         <v>44.48566715384414</v>
       </c>
-      <c r="G74" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H74" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G74" t="n">
+        <v>0.7389905560192176</v>
+      </c>
+      <c r="H74" t="n">
+        <v>1.214521679213109</v>
       </c>
       <c r="I74" t="n">
-        <v>0.7389905560192176</v>
-      </c>
-      <c r="J74" t="n">
-        <v>1.214521679213109</v>
-      </c>
-      <c r="K74" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.050266848392937</v>
+      </c>
+      <c r="J74" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K74" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L74" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M74" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -3819,25 +4413,33 @@
       <c r="F75" t="n">
         <v>33.22057870842356</v>
       </c>
-      <c r="G75" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H75" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G75" t="n">
+        <v>0.4893414053626657</v>
+      </c>
+      <c r="H75" t="n">
+        <v>1.335195887000838</v>
       </c>
       <c r="I75" t="n">
-        <v>0.4893414053626657</v>
-      </c>
-      <c r="J75" t="n">
-        <v>1.335195887000838</v>
-      </c>
-      <c r="K75" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.192637879111181</v>
+      </c>
+      <c r="J75" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K75" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L75" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M75" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -3864,23 +4466,31 @@
       <c r="F76" t="n">
         <v>84.3462463269766</v>
       </c>
-      <c r="G76" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H76" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
+      <c r="G76" t="n">
+        <v>2.81689846430919</v>
+      </c>
+      <c r="H76" t="n">
+        <v>2.232315855237073</v>
       </c>
       <c r="I76" t="n">
-        <v>2.81689846430919</v>
-      </c>
-      <c r="J76" t="n">
-        <v>2.232315855237073</v>
-      </c>
-      <c r="K76" s="3" t="inlineStr">
+        <v>1.37997593513003</v>
+      </c>
+      <c r="J76" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K76" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="L76" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M76" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -3909,25 +4519,33 @@
       <c r="F77" t="n">
         <v>69.77318220487415</v>
       </c>
-      <c r="G77" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H77" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G77" t="n">
+        <v>-0.4912301955781402</v>
+      </c>
+      <c r="H77" t="n">
+        <v>-1.418138314188866</v>
       </c>
       <c r="I77" t="n">
-        <v>-0.4912301955781402</v>
-      </c>
-      <c r="J77" t="n">
-        <v>-1.418138314188866</v>
-      </c>
-      <c r="K77" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.8668541520792189</v>
+      </c>
+      <c r="J77" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K77" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L77" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M77" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -3954,23 +4572,31 @@
       <c r="F78" t="n">
         <v>90.04324126709199</v>
       </c>
-      <c r="G78" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H78" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G78" t="n">
+        <v>4.917810278243735</v>
+      </c>
+      <c r="H78" t="n">
+        <v>2.722372155016304</v>
       </c>
       <c r="I78" t="n">
-        <v>4.917810278243735</v>
-      </c>
-      <c r="J78" t="n">
-        <v>2.722372155016304</v>
-      </c>
-      <c r="K78" s="3" t="inlineStr">
+        <v>1.021623460553715</v>
+      </c>
+      <c r="J78" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K78" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L78" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M78" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -3999,25 +4625,33 @@
       <c r="F79" t="n">
         <v>57.27554508644204</v>
       </c>
-      <c r="G79" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H79" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G79" t="n">
+        <v>0.8562482950337795</v>
+      </c>
+      <c r="H79" t="n">
+        <v>1.057216538504453</v>
       </c>
       <c r="I79" t="n">
-        <v>0.8562482950337795</v>
-      </c>
-      <c r="J79" t="n">
-        <v>1.057216538504453</v>
-      </c>
-      <c r="K79" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.198525753823551</v>
+      </c>
+      <c r="J79" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K79" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L79" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M79" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -4044,25 +4678,33 @@
       <c r="F80" t="n">
         <v>67.75279747870093</v>
       </c>
-      <c r="G80" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H80" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G80" t="n">
+        <v>2.018353410755054</v>
+      </c>
+      <c r="H80" t="n">
+        <v>2.524666829053764</v>
       </c>
       <c r="I80" t="n">
-        <v>2.018353410755054</v>
-      </c>
-      <c r="J80" t="n">
-        <v>2.524666829053764</v>
-      </c>
-      <c r="K80" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.252023161607436</v>
+      </c>
+      <c r="J80" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K80" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L80" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M80" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -4089,25 +4731,33 @@
       <c r="F81" t="n">
         <v>55.91939352970879</v>
       </c>
-      <c r="G81" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H81" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G81" t="n">
+        <v>-0.09570672156182521</v>
+      </c>
+      <c r="H81" t="n">
+        <v>-0.2707659894678785</v>
       </c>
       <c r="I81" t="n">
-        <v>-0.09570672156182521</v>
-      </c>
-      <c r="J81" t="n">
-        <v>-0.2707659894678785</v>
-      </c>
-      <c r="K81" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.8663319044309915</v>
+      </c>
+      <c r="J81" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K81" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L81" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M81" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -4134,25 +4784,33 @@
       <c r="F82" t="n">
         <v>51.03475149162225</v>
       </c>
-      <c r="G82" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H82" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G82" t="n">
+        <v>5.194550664614098</v>
+      </c>
+      <c r="H82" t="n">
+        <v>7.18372779402498</v>
       </c>
       <c r="I82" t="n">
-        <v>5.194550664614098</v>
-      </c>
-      <c r="J82" t="n">
-        <v>7.18372779402498</v>
-      </c>
-      <c r="K82" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.147309444410384</v>
+      </c>
+      <c r="J82" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K82" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L82" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M82" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -4179,23 +4837,31 @@
       <c r="F83" t="n">
         <v>86.91636649919367</v>
       </c>
-      <c r="G83" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H83" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G83" t="n">
+        <v>5.528207405485887</v>
+      </c>
+      <c r="H83" t="n">
+        <v>4.360941009092549</v>
       </c>
       <c r="I83" t="n">
-        <v>5.528207405485887</v>
-      </c>
-      <c r="J83" t="n">
-        <v>4.360941009092549</v>
-      </c>
-      <c r="K83" s="3" t="inlineStr">
+        <v>1.051596814893736</v>
+      </c>
+      <c r="J83" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K83" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L83" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M83" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -4224,25 +4890,33 @@
       <c r="F84" t="n">
         <v>53.18311994205096</v>
       </c>
-      <c r="G84" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H84" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G84" t="n">
+        <v>4.143613767114175</v>
+      </c>
+      <c r="H84" t="n">
+        <v>5.736051119302576</v>
       </c>
       <c r="I84" t="n">
-        <v>4.143613767114175</v>
-      </c>
-      <c r="J84" t="n">
-        <v>5.736051119302576</v>
-      </c>
-      <c r="K84" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.062013243507761</v>
+      </c>
+      <c r="J84" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K84" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L84" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M84" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -4269,25 +4943,33 @@
       <c r="F85" t="n">
         <v>60.69182767166736</v>
       </c>
-      <c r="G85" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H85" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G85" t="n">
+        <v>0.4747108610086883</v>
+      </c>
+      <c r="H85" t="n">
+        <v>0.5302958324488527</v>
       </c>
       <c r="I85" t="n">
-        <v>0.4747108610086883</v>
-      </c>
-      <c r="J85" t="n">
-        <v>0.5302958324488527</v>
-      </c>
-      <c r="K85" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.132914648197491</v>
+      </c>
+      <c r="J85" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K85" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L85" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M85" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -4314,25 +4996,33 @@
       <c r="F86" t="n">
         <v>62.30000480652222</v>
       </c>
-      <c r="G86" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H86" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G86" t="n">
+        <v>0.7178614815438493</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0.9575689596086456</v>
       </c>
       <c r="I86" t="n">
-        <v>0.7178614815438493</v>
-      </c>
-      <c r="J86" t="n">
-        <v>0.9575689596086456</v>
-      </c>
-      <c r="K86" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.072479595527054</v>
+      </c>
+      <c r="J86" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K86" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L86" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M86" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -4359,25 +5049,33 @@
       <c r="F87" t="n">
         <v>54.64359606609416</v>
       </c>
-      <c r="G87" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H87" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G87" t="n">
+        <v>2.613104895605716</v>
+      </c>
+      <c r="H87" t="n">
+        <v>3.959895340985105</v>
       </c>
       <c r="I87" t="n">
-        <v>2.613104895605716</v>
-      </c>
-      <c r="J87" t="n">
-        <v>3.959895340985105</v>
-      </c>
-      <c r="K87" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.119945781355956</v>
+      </c>
+      <c r="J87" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K87" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L87" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M87" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -4404,23 +5102,31 @@
       <c r="F88" t="n">
         <v>81.61072033102208</v>
       </c>
-      <c r="G88" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H88" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G88" t="n">
+        <v>9.577140131840141</v>
+      </c>
+      <c r="H88" t="n">
+        <v>6.311552747906563</v>
       </c>
       <c r="I88" t="n">
-        <v>9.577140131840141</v>
-      </c>
-      <c r="J88" t="n">
-        <v>6.311552747906563</v>
-      </c>
-      <c r="K88" s="3" t="inlineStr">
+        <v>1.284717985383394</v>
+      </c>
+      <c r="J88" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K88" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L88" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M88" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -4449,23 +5155,31 @@
       <c r="F89" t="n">
         <v>83.02882375681868</v>
       </c>
-      <c r="G89" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H89" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G89" t="n">
+        <v>3.751637154967796</v>
+      </c>
+      <c r="H89" t="n">
+        <v>1.726674624498964</v>
       </c>
       <c r="I89" t="n">
-        <v>3.751637154967796</v>
-      </c>
-      <c r="J89" t="n">
-        <v>1.726674624498964</v>
-      </c>
-      <c r="K89" s="3" t="inlineStr">
+        <v>1.07490940944333</v>
+      </c>
+      <c r="J89" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K89" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L89" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M89" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -4494,23 +5208,31 @@
       <c r="F90" t="n">
         <v>64.65624720690914</v>
       </c>
-      <c r="G90" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H90" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G90" t="n">
+        <v>1.217791864307799</v>
+      </c>
+      <c r="H90" t="n">
+        <v>0.6859463089662597</v>
       </c>
       <c r="I90" t="n">
-        <v>1.217791864307799</v>
-      </c>
-      <c r="J90" t="n">
-        <v>0.6859463089662597</v>
-      </c>
-      <c r="K90" s="3" t="inlineStr">
+        <v>1.075720947000318</v>
+      </c>
+      <c r="J90" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K90" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L90" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M90" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -4539,23 +5261,31 @@
       <c r="F91" t="n">
         <v>68.83940368701008</v>
       </c>
-      <c r="G91" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H91" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G91" t="n">
+        <v>1.585683888102324</v>
+      </c>
+      <c r="H91" t="n">
+        <v>1.047465076526539</v>
       </c>
       <c r="I91" t="n">
-        <v>1.585683888102324</v>
-      </c>
-      <c r="J91" t="n">
-        <v>1.047465076526539</v>
-      </c>
-      <c r="K91" s="3" t="inlineStr">
+        <v>1.055173391846352</v>
+      </c>
+      <c r="J91" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K91" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L91" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M91" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -4584,25 +5314,33 @@
       <c r="F92" t="n">
         <v>29.90355127388571</v>
       </c>
-      <c r="G92" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
-        </is>
-      </c>
-      <c r="H92" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G92" t="n">
+        <v>-0.8034101086968803</v>
+      </c>
+      <c r="H92" t="n">
+        <v>2.115380797855594</v>
       </c>
       <c r="I92" t="n">
-        <v>-0.8034101086968803</v>
-      </c>
-      <c r="J92" t="n">
-        <v>2.115380797855594</v>
-      </c>
-      <c r="K92" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.128716149974424</v>
+      </c>
+      <c r="J92" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="K92" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L92" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M92" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -4629,25 +5367,33 @@
       <c r="F93" t="n">
         <v>40.67598347321289</v>
       </c>
-      <c r="G93" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H93" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G93" t="n">
+        <v>0.00075089208309</v>
+      </c>
+      <c r="H93" t="n">
+        <v>1.231133358217463</v>
       </c>
       <c r="I93" t="n">
-        <v>0.00075089208309</v>
-      </c>
-      <c r="J93" t="n">
-        <v>1.231133358217463</v>
-      </c>
-      <c r="K93" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.075002217063125</v>
+      </c>
+      <c r="J93" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K93" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L93" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M93" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -4674,25 +5420,33 @@
       <c r="F94" t="n">
         <v>66.05656921102441</v>
       </c>
-      <c r="G94" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H94" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G94" t="n">
+        <v>0.5799773642821151</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0.1174463027301929</v>
       </c>
       <c r="I94" t="n">
-        <v>0.5799773642821151</v>
-      </c>
-      <c r="J94" t="n">
-        <v>0.1174463027301929</v>
-      </c>
-      <c r="K94" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.9742783769421366</v>
+      </c>
+      <c r="J94" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K94" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L94" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M94" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -4719,25 +5473,33 @@
       <c r="F95" t="n">
         <v>41.86441664242072</v>
       </c>
-      <c r="G95" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H95" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G95" t="n">
+        <v>1.653099650098</v>
+      </c>
+      <c r="H95" t="n">
+        <v>4.047659658168035</v>
       </c>
       <c r="I95" t="n">
-        <v>1.653099650098</v>
-      </c>
-      <c r="J95" t="n">
-        <v>4.047659658168035</v>
-      </c>
-      <c r="K95" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.035127828619737</v>
+      </c>
+      <c r="J95" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K95" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L95" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M95" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -4764,23 +5526,31 @@
       <c r="F96" t="n">
         <v>90.21226359183945</v>
       </c>
-      <c r="G96" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H96" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G96" t="n">
+        <v>5.497703403898868</v>
+      </c>
+      <c r="H96" t="n">
+        <v>4.229622071197362</v>
       </c>
       <c r="I96" t="n">
-        <v>5.497703403898868</v>
-      </c>
-      <c r="J96" t="n">
-        <v>4.229622071197362</v>
-      </c>
-      <c r="K96" s="3" t="inlineStr">
+        <v>1.055125681432928</v>
+      </c>
+      <c r="J96" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K96" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L96" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M96" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -4809,23 +5579,31 @@
       <c r="F97" t="n">
         <v>78.58315815273235</v>
       </c>
-      <c r="G97" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="H97" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G97" t="n">
+        <v>0.8658363714916746</v>
+      </c>
+      <c r="H97" t="n">
+        <v>0.827181565714825</v>
       </c>
       <c r="I97" t="n">
-        <v>0.8658363714916746</v>
-      </c>
-      <c r="J97" t="n">
-        <v>0.827181565714825</v>
-      </c>
-      <c r="K97" s="3" t="inlineStr">
+        <v>1.081959192915911</v>
+      </c>
+      <c r="J97" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="K97" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L97" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M97" s="3" t="inlineStr">
         <is>
           <t>Buy</t>
         </is>
@@ -4854,25 +5632,33 @@
       <c r="F98" t="n">
         <v>58.36248858126906</v>
       </c>
-      <c r="G98" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H98" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G98" t="n">
+        <v>-0.2807676118431743</v>
+      </c>
+      <c r="H98" t="n">
+        <v>-0.4349451546214669</v>
       </c>
       <c r="I98" t="n">
-        <v>-0.2807676118431743</v>
-      </c>
-      <c r="J98" t="n">
-        <v>-0.4349451546214669</v>
-      </c>
-      <c r="K98" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.9494864450104221</v>
+      </c>
+      <c r="J98" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K98" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L98" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M98" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>
@@ -4899,25 +5685,33 @@
       <c r="F99" t="n">
         <v>63.42061559592932</v>
       </c>
-      <c r="G99" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H99" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G99" t="n">
+        <v>1.759008151029121</v>
+      </c>
+      <c r="H99" t="n">
+        <v>1.865074296388382</v>
       </c>
       <c r="I99" t="n">
-        <v>1.759008151029121</v>
-      </c>
-      <c r="J99" t="n">
-        <v>1.865074296388382</v>
-      </c>
-      <c r="K99" s="4" t="inlineStr">
-        <is>
-          <t>Sell</t>
+        <v>1.180327857769425</v>
+      </c>
+      <c r="J99" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K99" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L99" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
+        </is>
+      </c>
+      <c r="M99" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
         </is>
       </c>
     </row>
@@ -4944,25 +5738,33 @@
       <c r="F100" t="n">
         <v>50.37244781255284</v>
       </c>
-      <c r="G100" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
-      </c>
-      <c r="H100" s="2" t="inlineStr">
-        <is>
-          <t>Hold</t>
-        </is>
+      <c r="G100" t="n">
+        <v>-0.2036852952601151</v>
+      </c>
+      <c r="H100" t="n">
+        <v>-0.4203760588456724</v>
       </c>
       <c r="I100" t="n">
-        <v>-0.2036852952601151</v>
-      </c>
-      <c r="J100" t="n">
-        <v>-0.4203760588456724</v>
-      </c>
-      <c r="K100" s="3" t="inlineStr">
-        <is>
-          <t>Buy</t>
+        <v>0.9798471191845665</v>
+      </c>
+      <c r="J100" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="K100" s="2" t="inlineStr">
+        <is>
+          <t>Hold</t>
+        </is>
+      </c>
+      <c r="L100" s="3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="M100" s="4" t="inlineStr">
+        <is>
+          <t>Sell</t>
         </is>
       </c>
     </row>

</xml_diff>